<commit_message>
small changes, implicit to explicit in main
</commit_message>
<xml_diff>
--- a/productionProfile.xlsx
+++ b/productionProfile.xlsx
@@ -585,19 +585,19 @@
         <v>0.02703703703703704</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9618545030951203</v>
+        <v>0.9628038282203389</v>
       </c>
       <c r="G3" t="n">
-        <v>266.9765070312308</v>
+        <v>268.5377777777778</v>
       </c>
       <c r="H3" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I3" t="n">
-        <v>262.7817213665642</v>
+        <v>264.3677663248773</v>
       </c>
       <c r="J3" t="n">
-        <v>236.8473604063308</v>
+        <v>238.3541611133802</v>
       </c>
       <c r="K3" t="n">
         <v>82.10493911391669</v>
@@ -612,13 +612,13 @@
         <v>6666666.666666667</v>
       </c>
       <c r="O3" t="n">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="P3" t="n">
-        <v>0.3466576067094818</v>
+        <v>0.3444661453796103</v>
       </c>
       <c r="Q3" t="n">
-        <v>49940214.62888516</v>
+        <v>50248814.5920181</v>
       </c>
     </row>
     <row r="4">
@@ -638,19 +638,19 @@
         <v>0.05407407407407407</v>
       </c>
       <c r="F4" t="n">
-        <v>0.956691536800344</v>
+        <v>0.957632213120615</v>
       </c>
       <c r="G4" t="n">
-        <v>258.1644368804317</v>
+        <v>259.8138465509401</v>
       </c>
       <c r="H4" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I4" t="n">
-        <v>253.8240616008817</v>
+        <v>255.5014924366847</v>
       </c>
       <c r="J4" t="n">
-        <v>228.3277104965653</v>
+        <v>229.9243981674038</v>
       </c>
       <c r="K4" t="n">
         <v>82.10493911391669</v>
@@ -665,13 +665,13 @@
         <v>6666666.666666667</v>
       </c>
       <c r="O4" t="n">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="P4" t="n">
-        <v>0.3595925301197804</v>
+        <v>0.3570953746898037</v>
       </c>
       <c r="Q4" t="n">
-        <v>48197964.36271162</v>
+        <v>48524133.73846352</v>
       </c>
     </row>
     <row r="5">
@@ -691,19 +691,19 @@
         <v>0.08111111111111111</v>
       </c>
       <c r="F5" t="n">
-        <v>0.951978205953497</v>
+        <v>0.9527648263123382</v>
       </c>
       <c r="G5" t="n">
-        <v>249.5498778584393</v>
+        <v>251.0320092655882</v>
       </c>
       <c r="H5" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I5" t="n">
-        <v>245.0569715738358</v>
+        <v>246.5661117300918</v>
       </c>
       <c r="J5" t="n">
-        <v>219.9722946275802</v>
+        <v>221.4118536136745</v>
       </c>
       <c r="K5" t="n">
         <v>82.10493911391669</v>
@@ -718,13 +718,13 @@
         <v>6666666.666666667</v>
       </c>
       <c r="O5" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="P5" t="n">
-        <v>0.3732512735429834</v>
+        <v>0.3708244964028694</v>
       </c>
       <c r="Q5" t="n">
-        <v>46493948.71996737</v>
+        <v>46787185.0623178</v>
       </c>
     </row>
     <row r="6">
@@ -744,19 +744,19 @@
         <v>0.1081481481481481</v>
       </c>
       <c r="F6" t="n">
-        <v>0.947702706905829</v>
+        <v>0.9483336191030337</v>
       </c>
       <c r="G6" t="n">
-        <v>241.1194226305332</v>
+        <v>242.4073532227854</v>
       </c>
       <c r="H6" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I6" t="n">
-        <v>236.4663903125759</v>
+        <v>237.7795253470198</v>
       </c>
       <c r="J6" t="n">
-        <v>211.7668360895158</v>
+        <v>213.0223568079941</v>
       </c>
       <c r="K6" t="n">
         <v>82.10493911391669</v>
@@ -771,13 +771,13 @@
         <v>6666666.666666667</v>
       </c>
       <c r="O6" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="P6" t="n">
-        <v>0.38771386790333</v>
+        <v>0.3854287425235901</v>
       </c>
       <c r="Q6" t="n">
-        <v>44825484.23424003</v>
+        <v>45080436.60574412</v>
       </c>
     </row>
     <row r="7">
@@ -797,19 +797,19 @@
         <v>0.1351851851851852</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9438537148925394</v>
+        <v>0.944348726724182</v>
       </c>
       <c r="G7" t="n">
-        <v>232.8601461772526</v>
+        <v>233.9653928196675</v>
       </c>
       <c r="H7" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I7" t="n">
-        <v>228.0386490388619</v>
+        <v>229.1671503838172</v>
       </c>
       <c r="J7" t="n">
-        <v>203.6972266438081</v>
+        <v>204.7789878284609</v>
       </c>
       <c r="K7" t="n">
         <v>82.10493911391669</v>
@@ -824,13 +824,13 @@
         <v>6666666.666666667</v>
       </c>
       <c r="O7" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="P7" t="n">
-        <v>0.4030734265100634</v>
+        <v>0.4009441592840292</v>
       </c>
       <c r="Q7" t="n">
-        <v>43189975.34334401</v>
+        <v>43408893.70110909</v>
       </c>
     </row>
     <row r="8">
@@ -850,19 +850,19 @@
         <v>0.1622222222222222</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9404203721463003</v>
+        <v>0.9408005008012981</v>
       </c>
       <c r="G8" t="n">
-        <v>224.7595844852474</v>
+        <v>225.6984575347756</v>
       </c>
       <c r="H8" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I8" t="n">
-        <v>219.7604345549008</v>
+        <v>220.720573375829</v>
       </c>
       <c r="J8" t="n">
-        <v>195.7494543980708</v>
+        <v>196.6724345223913</v>
       </c>
       <c r="K8" t="n">
         <v>82.10493911391669</v>
@@ -877,13 +877,13 @@
         <v>6666666.666666667</v>
       </c>
       <c r="O8" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="P8" t="n">
-        <v>0.4194389167846685</v>
+        <v>0.4174704976490692</v>
       </c>
       <c r="Q8" t="n">
-        <v>41584909.09025044</v>
+        <v>41770993.34343581</v>
       </c>
     </row>
     <row r="9">
@@ -903,19 +903,19 @@
         <v>0.1892592592592593</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9373922766341799</v>
+        <v>0.9376768302785298</v>
       </c>
       <c r="G9" t="n">
-        <v>216.8057139323989</v>
+        <v>217.5939884810724</v>
       </c>
       <c r="H9" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I9" t="n">
-        <v>211.6187500471425</v>
+        <v>212.4262733300164</v>
       </c>
       <c r="J9" t="n">
-        <v>187.9095196371167</v>
+        <v>188.6882258919396</v>
       </c>
       <c r="K9" t="n">
         <v>82.10493911391669</v>
@@ -930,13 +930,13 @@
         <v>6666666.666666667</v>
       </c>
       <c r="O9" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="P9" t="n">
-        <v>0.4369386887501732</v>
+        <v>0.4351354660620828</v>
       </c>
       <c r="Q9" t="n">
-        <v>40007849.73194604</v>
+        <v>40164195.61889236</v>
       </c>
     </row>
     <row r="10">
@@ -956,19 +956,19 @@
         <v>0.2162962962962963</v>
       </c>
       <c r="F10" t="n">
-        <v>0.934759471413329</v>
+        <v>0.9349657784599498</v>
       </c>
       <c r="G10" t="n">
-        <v>208.9869313325153</v>
+        <v>209.6391738563736</v>
       </c>
       <c r="H10" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I10" t="n">
-        <v>203.6008724086398</v>
+        <v>204.270313538117</v>
       </c>
       <c r="J10" t="n">
-        <v>180.1633347321442</v>
+        <v>180.8111382189398</v>
       </c>
       <c r="K10" t="n">
         <v>82.10493911391669</v>
@@ -983,13 +983,13 @@
         <v>6666666.666666667</v>
       </c>
       <c r="O10" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P10" t="n">
-        <v>0.4557250188335229</v>
+        <v>0.4540922640202498</v>
       </c>
       <c r="Q10" t="n">
-        <v>38456433.19204319</v>
+        <v>38585898.76303797</v>
       </c>
     </row>
     <row r="11">
@@ -1009,19 +1009,19 @@
         <v>0.2433333333333333</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9325124346037983</v>
+        <v>0.9326559295528546</v>
       </c>
       <c r="G11" t="n">
-        <v>201.2920346058478</v>
+        <v>201.8216131487897</v>
       </c>
       <c r="H11" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I11" t="n">
-        <v>195.6943049082922</v>
+        <v>196.2389902943794</v>
       </c>
       <c r="J11" t="n">
-        <v>172.4966028277356</v>
+        <v>173.025737359659</v>
       </c>
       <c r="K11" t="n">
         <v>82.10493911391669</v>
@@ -1036,13 +1036,13 @@
         <v>6666666.666666667</v>
       </c>
       <c r="O11" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="P11" t="n">
-        <v>0.4759800353628477</v>
+        <v>0.4745244283701545</v>
       </c>
       <c r="Q11" t="n">
-        <v>36928361.27604014</v>
+        <v>37033568.62028682</v>
       </c>
     </row>
     <row r="12">
@@ -1062,19 +1062,19 @@
         <v>0.2703703703703704</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9306420699802572</v>
+        <v>0.9307364170666969</v>
       </c>
       <c r="G12" t="n">
-        <v>193.7102040424555</v>
+        <v>194.1293825443784</v>
       </c>
       <c r="H12" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I12" t="n">
-        <v>187.8867236606874</v>
+        <v>188.3188650795225</v>
       </c>
       <c r="J12" t="n">
-        <v>164.8946679487507</v>
+        <v>165.3163100648555</v>
       </c>
       <c r="K12" t="n">
         <v>82.10493911391669</v>
@@ -1092,10 +1092,10 @@
         <v>83</v>
       </c>
       <c r="P12" t="n">
-        <v>0.4979235540802018</v>
+        <v>0.4966535914194189</v>
       </c>
       <c r="Q12" t="n">
-        <v>35421395.54518942</v>
+        <v>35504749.1733817</v>
       </c>
     </row>
     <row r="13">
@@ -1115,19 +1115,19 @@
         <v>0.2974074074074074</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9291396981882016</v>
+        <v>0.9291969136531754</v>
       </c>
       <c r="G13" t="n">
-        <v>186.2309841261573</v>
+        <v>186.5510205304728</v>
       </c>
       <c r="H13" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I13" t="n">
-        <v>180.1659158286462</v>
+        <v>180.496706448452</v>
       </c>
       <c r="J13" t="n">
-        <v>157.3423261382571</v>
+        <v>157.6666774884208</v>
       </c>
       <c r="K13" t="n">
         <v>82.10493911391669</v>
@@ -1142,13 +1142,13 @@
         <v>6666666.666666667</v>
       </c>
       <c r="O13" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="P13" t="n">
-        <v>0.521823600356403</v>
+        <v>0.5207501066288821</v>
       </c>
       <c r="Q13" t="n">
-        <v>33933350.71355318</v>
+        <v>33997056.68190652</v>
       </c>
     </row>
     <row r="14">
@@ -1168,19 +1168,19 @@
         <v>0.3244444444444444</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9279970485946986</v>
+        <v>0.9280276173484514</v>
       </c>
       <c r="G14" t="n">
-        <v>178.844265887259</v>
+        <v>179.075504753667</v>
       </c>
       <c r="H14" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I14" t="n">
-        <v>172.5197067541281</v>
+        <v>172.7594112647945</v>
       </c>
       <c r="J14" t="n">
-        <v>149.8235826812256</v>
+        <v>150.0599450122607</v>
       </c>
       <c r="K14" t="n">
         <v>82.10493911391669</v>
@@ -1198,10 +1198,10 @@
         <v>68</v>
       </c>
       <c r="P14" t="n">
-        <v>0.5480107847147703</v>
+        <v>0.5471476022945914</v>
       </c>
       <c r="Q14" t="n">
-        <v>32462087.3893895</v>
+        <v>32508171.32180775</v>
       </c>
     </row>
     <row r="15">
@@ -1221,19 +1221,19 @@
         <v>0.3514814814814815</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9272062517888042</v>
+        <v>0.9272192380633747</v>
       </c>
       <c r="G15" t="n">
-        <v>171.5402697526128</v>
+        <v>171.69222868235</v>
       </c>
       <c r="H15" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I15" t="n">
-        <v>164.9358721581723</v>
+        <v>165.0939101471951</v>
       </c>
       <c r="J15" t="n">
-        <v>142.3213334625894</v>
+        <v>142.4781745152127</v>
       </c>
       <c r="K15" t="n">
         <v>82.10493911391669</v>
@@ -1251,10 +1251,10 @@
         <v>60</v>
       </c>
       <c r="P15" t="n">
-        <v>0.5768983265990744</v>
+        <v>0.576263272555827</v>
       </c>
       <c r="Q15" t="n">
-        <v>31005503.92122373</v>
+        <v>31035827.78419731</v>
       </c>
     </row>
     <row r="16">
@@ -1274,19 +1274,19 @@
         <v>0.3785185185185185</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9267598327529669</v>
+        <v>0.9267629847293799</v>
       </c>
       <c r="G16" t="n">
-        <v>164.3095288617068</v>
+        <v>164.3909789498979</v>
       </c>
       <c r="H16" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I16" t="n">
-        <v>157.4020300140181</v>
+        <v>157.4870526039635</v>
       </c>
       <c r="J16" t="n">
-        <v>134.8169374570568</v>
+        <v>134.9019464625157</v>
       </c>
       <c r="K16" t="n">
         <v>82.10493911391669</v>
@@ -1304,10 +1304,10 @@
         <v>53</v>
       </c>
       <c r="P16" t="n">
-        <v>0.6090105639736072</v>
+        <v>0.60862679351132</v>
       </c>
       <c r="Q16" t="n">
-        <v>29561527.02269334</v>
+        <v>29577804.68478708</v>
       </c>
     </row>
     <row r="17">
@@ -1327,19 +1327,19 @@
         <v>0.4055555555555556</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9266507047339156</v>
+        <v>0.9266505531855013</v>
       </c>
       <c r="G17" t="n">
-        <v>157.14287281739</v>
+        <v>157.1619134342665</v>
       </c>
       <c r="H17" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I17" t="n">
-        <v>149.9055044188844</v>
+        <v>149.9254641883682</v>
       </c>
       <c r="J17" t="n">
-        <v>127.2896294055521</v>
+        <v>127.3097601115605</v>
       </c>
       <c r="K17" t="n">
         <v>82.10493911391669</v>
@@ -1357,10 +1357,10 @@
         <v>45</v>
       </c>
       <c r="P17" t="n">
-        <v>0.6450245750368681</v>
+        <v>0.6449225812849604</v>
       </c>
       <c r="Q17" t="n">
-        <v>28128100.72604998</v>
+        <v>28131912.34743676</v>
       </c>
     </row>
     <row r="18">
@@ -1380,19 +1380,19 @@
         <v>0.4325925925925926</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9268721638504166</v>
+        <v>0.9268741148711429</v>
       </c>
       <c r="G18" t="n">
-        <v>150.0314118395185</v>
+        <v>149.9955400524127</v>
       </c>
       <c r="H18" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I18" t="n">
-        <v>142.4331503419657</v>
+        <v>142.3953644378662</v>
       </c>
       <c r="J18" t="n">
-        <v>119.7156916234817</v>
+        <v>119.6771893470906</v>
       </c>
       <c r="K18" t="n">
         <v>82.10493911391669</v>
@@ -1410,10 +1410,10 @@
         <v>38</v>
       </c>
       <c r="P18" t="n">
-        <v>0.6858327258564003</v>
+        <v>0.6860533704196046</v>
       </c>
       <c r="Q18" t="n">
-        <v>26703173.03246218</v>
+        <v>26695978.32666857</v>
       </c>
     </row>
     <row r="19">
@@ -1433,19 +1433,19 @@
         <v>0.4596296296296296</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9274178844860644</v>
+        <v>0.92742630639449</v>
       </c>
       <c r="G19" t="n">
-        <v>142.9665212891631</v>
+        <v>142.8826962394972</v>
       </c>
       <c r="H19" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I19" t="n">
-        <v>134.9711227904047</v>
+        <v>134.8823289480361</v>
       </c>
       <c r="J19" t="n">
-        <v>112.0672513919107</v>
+        <v>111.975658034495</v>
       </c>
       <c r="K19" t="n">
         <v>82.10493911391669</v>
@@ -1463,10 +1463,10 @@
         <v>30</v>
       </c>
       <c r="P19" t="n">
-        <v>0.7326398934046066</v>
+        <v>0.7332391749698278</v>
       </c>
       <c r="Q19" t="n">
-        <v>25284679.35653578</v>
+        <v>25267829.75923455</v>
       </c>
     </row>
     <row r="20">
@@ -1486,19 +1486,19 @@
         <v>0.4866666666666667</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9282819155287133</v>
+        <v>0.9283002200559735</v>
       </c>
       <c r="G20" t="n">
-        <v>135.9398265300127</v>
+        <v>135.8145290795977</v>
       </c>
       <c r="H20" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I20" t="n">
-        <v>127.504565466448</v>
+        <v>127.3709703460355</v>
       </c>
       <c r="J20" t="n">
-        <v>104.3104746834127</v>
+        <v>104.1706008543322</v>
       </c>
       <c r="K20" t="n">
         <v>82.10493911391669</v>
@@ -1516,10 +1516,10 @@
         <v>22</v>
       </c>
       <c r="P20" t="n">
-        <v>0.7871207504625887</v>
+        <v>0.7881776474413239</v>
       </c>
       <c r="Q20" t="n">
-        <v>23870521.45112526</v>
+        <v>23845271.21912915</v>
       </c>
     </row>
     <row r="21">
@@ -1539,19 +1539,19 @@
         <v>0.5137037037037037</v>
       </c>
       <c r="F21" t="n">
-        <v>0.929458677535088</v>
+        <v>0.9294893954191565</v>
       </c>
       <c r="G21" t="n">
-        <v>128.9431880921711</v>
+        <v>128.7824760516721</v>
       </c>
       <c r="H21" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I21" t="n">
-        <v>120.017180158304</v>
+        <v>119.8444988966005</v>
       </c>
       <c r="J21" t="n">
-        <v>96.40274301406612</v>
+        <v>96.21858693449948</v>
       </c>
       <c r="K21" t="n">
         <v>82.10493911391669</v>
@@ -1569,10 +1569,10 @@
         <v>14</v>
       </c>
       <c r="P21" t="n">
-        <v>0.8516867523358413</v>
+        <v>0.8533168250517894</v>
       </c>
       <c r="Q21" t="n">
-        <v>22458539.85960756</v>
+        <v>22426056.10492486</v>
       </c>
     </row>
     <row r="22">
@@ -1592,19 +1592,19 @@
         <v>0.5407407407407407</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9309429609206826</v>
+        <v>0.9309878120390673</v>
       </c>
       <c r="G22" t="n">
-        <v>121.9686871014738</v>
+        <v>121.7782463513104</v>
       </c>
       <c r="H22" t="n">
         <v>2222222.222222222</v>
       </c>
       <c r="I22" t="n">
-        <v>112.4906147686774</v>
+        <v>112.2840997745371</v>
       </c>
       <c r="J22" t="n">
-        <v>88.28802320635332</v>
+        <v>88.06259595762397</v>
       </c>
       <c r="K22" t="n">
         <v>82.10493911391669</v>
@@ -1622,10 +1622,10 @@
         <v>6</v>
       </c>
       <c r="P22" t="n">
-        <v>0.9299668984774405</v>
+        <v>0.9323474764862243</v>
       </c>
       <c r="Q22" t="n">
-        <v>21046476.92557138</v>
+        <v>21007848.56039558</v>
       </c>
     </row>
     <row r="23">
@@ -1633,7 +1633,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>19631925.72471662</v>
+        <v>19588171.24610576</v>
       </c>
       <c r="C23" t="n">
         <v>7300000000</v>
@@ -1645,40 +1645,40 @@
         <v>0.5677777777777778</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9327299253030228</v>
+        <v>0.9327898834818611</v>
       </c>
       <c r="G23" t="n">
-        <v>115.0086109348212</v>
+        <v>114.7938027452871</v>
       </c>
       <c r="H23" t="n">
-        <v>2181325.080524069</v>
+        <v>2176463.47178953</v>
       </c>
       <c r="I23" t="n">
-        <v>105.0983135384817</v>
+        <v>104.8863846117996</v>
       </c>
       <c r="J23" t="n">
-        <v>80.79727167080664</v>
+        <v>80.64204529660928</v>
       </c>
       <c r="K23" t="n">
-        <v>80.79727167080662</v>
+        <v>80.6420452966093</v>
       </c>
       <c r="L23" t="n">
-        <v>77.42078463722542</v>
+        <v>77.27416697633325</v>
       </c>
       <c r="M23" t="n">
         <v>30</v>
       </c>
       <c r="N23" t="n">
-        <v>6543975.241572208</v>
+        <v>6529390.415368588</v>
       </c>
       <c r="O23" t="n">
         <v>0</v>
       </c>
       <c r="P23" t="n">
-        <v>0.9999999999999998</v>
+        <v>1</v>
       </c>
       <c r="Q23" t="n">
-        <v>19631925.72471662</v>
+        <v>19588171.24610576</v>
       </c>
     </row>
     <row r="24">
@@ -1686,52 +1686,52 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>18238447.87785159</v>
+        <v>18194662.73762699</v>
       </c>
       <c r="C24" t="n">
-        <v>7165652889.521567</v>
+        <v>7149682504.828604</v>
       </c>
       <c r="D24" t="n">
-        <v>160465652889.5216</v>
+        <v>160449682504.8286</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5943172329241539</v>
+        <v>0.5942580833512171</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9347740566338306</v>
+        <v>0.934842726767572</v>
       </c>
       <c r="G24" t="n">
-        <v>108.1833849451009</v>
+        <v>107.9694923062597</v>
       </c>
       <c r="H24" t="n">
-        <v>2026494.208650177</v>
+        <v>2021629.193069666</v>
       </c>
       <c r="I24" t="n">
-        <v>98.37250921639499</v>
+        <v>98.1620195177432</v>
       </c>
       <c r="J24" t="n">
-        <v>75.87867771293824</v>
+        <v>75.72501911922294</v>
       </c>
       <c r="K24" t="n">
-        <v>75.87867771293824</v>
+        <v>75.72501911922292</v>
       </c>
       <c r="L24" t="n">
-        <v>72.77705172311555</v>
+        <v>72.63205351121533</v>
       </c>
       <c r="M24" t="n">
         <v>30</v>
       </c>
       <c r="N24" t="n">
-        <v>6079482.62595053</v>
+        <v>6064887.579208997</v>
       </c>
       <c r="O24" t="n">
         <v>0</v>
       </c>
       <c r="P24" t="n">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="Q24" t="n">
-        <v>18238447.87785159</v>
+        <v>18194662.73762699</v>
       </c>
     </row>
     <row r="25">
@@ -1739,43 +1739,43 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>16937025.43237332</v>
+        <v>16896880.81813582</v>
       </c>
       <c r="C25" t="n">
-        <v>6657033475.415831</v>
+        <v>6641051899.233852</v>
       </c>
       <c r="D25" t="n">
-        <v>167122686364.9374</v>
+        <v>167090734404.0625</v>
       </c>
       <c r="E25" t="n">
-        <v>0.6189729124627311</v>
+        <v>0.6188545718668981</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9369271609926162</v>
+        <v>0.9369972037733888</v>
       </c>
       <c r="G25" t="n">
-        <v>101.8424962540803</v>
+        <v>101.6474817538715</v>
       </c>
       <c r="H25" t="n">
-        <v>1881891.714708147</v>
+        <v>1877431.202015091</v>
       </c>
       <c r="I25" t="n">
-        <v>92.14120863410797</v>
+        <v>91.94987408848661</v>
       </c>
       <c r="J25" t="n">
-        <v>71.33773891381587</v>
+        <v>71.1985843266297</v>
       </c>
       <c r="K25" t="n">
-        <v>71.33773891381587</v>
+        <v>71.19858432662973</v>
       </c>
       <c r="L25" t="n">
-        <v>68.49417292940845</v>
+        <v>68.36300033256367</v>
       </c>
       <c r="M25" t="n">
         <v>30</v>
       </c>
       <c r="N25" t="n">
-        <v>5645675.144124441</v>
+        <v>5632293.606045272</v>
       </c>
       <c r="O25" t="n">
         <v>0</v>
@@ -1784,7 +1784,7 @@
         <v>1</v>
       </c>
       <c r="Q25" t="n">
-        <v>16937025.43237332</v>
+        <v>16896880.81813582</v>
       </c>
     </row>
     <row r="26">
@@ -1792,43 +1792,43 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>15720251.99604272</v>
+        <v>15684391.11255466</v>
       </c>
       <c r="C26" t="n">
-        <v>6182014282.816263</v>
+        <v>6167361498.619573</v>
       </c>
       <c r="D26" t="n">
-        <v>173304700647.7537</v>
+        <v>173258095902.682</v>
       </c>
       <c r="E26" t="n">
-        <v>0.6418692616583469</v>
+        <v>0.641696651491415</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9391432186378683</v>
+        <v>0.939211396526126</v>
       </c>
       <c r="G26" t="n">
-        <v>95.94907240131801</v>
+        <v>95.77596076110649</v>
       </c>
       <c r="H26" t="n">
-        <v>1746694.666226969</v>
+        <v>1742710.123617184</v>
       </c>
       <c r="I26" t="n">
-        <v>86.36856967929013</v>
+        <v>86.1993302531744</v>
       </c>
       <c r="J26" t="n">
-        <v>67.14758880911711</v>
+        <v>67.02501585728167</v>
       </c>
       <c r="K26" t="n">
-        <v>67.14758880911712</v>
+        <v>67.02501585728167</v>
       </c>
       <c r="L26" t="n">
-        <v>64.5465435550426</v>
+        <v>64.4311367184182</v>
       </c>
       <c r="M26" t="n">
         <v>30</v>
       </c>
       <c r="N26" t="n">
-        <v>5240083.998680907</v>
+        <v>5228130.370851552</v>
       </c>
       <c r="O26" t="n">
         <v>0</v>
@@ -1837,7 +1837,7 @@
         <v>1</v>
       </c>
       <c r="Q26" t="n">
-        <v>15720251.99604272</v>
+        <v>15684391.11255466</v>
       </c>
     </row>
     <row r="27">
@@ -1845,43 +1845,43 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>14581640.59829105</v>
+        <v>14550421.74583181</v>
       </c>
       <c r="C27" t="n">
-        <v>5737891978.555593</v>
+        <v>5724802756.08245</v>
       </c>
       <c r="D27" t="n">
-        <v>179042592626.3093</v>
+        <v>178982898658.7645</v>
       </c>
       <c r="E27" t="n">
-        <v>0.6631207134307751</v>
+        <v>0.6628996246620907</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9413848475044799</v>
+        <v>0.9414484986958492</v>
       </c>
       <c r="G27" t="n">
-        <v>90.47089107522415</v>
+        <v>90.32125123732938</v>
       </c>
       <c r="H27" t="n">
-        <v>1620182.288699005</v>
+        <v>1616713.527314645</v>
       </c>
       <c r="I27" t="n">
-        <v>81.02345242734394</v>
+        <v>80.87777752734139</v>
       </c>
       <c r="J27" t="n">
-        <v>63.28477692818519</v>
+        <v>63.17975909350497</v>
       </c>
       <c r="K27" t="n">
-        <v>63.28477692818518</v>
+        <v>63.17975909350496</v>
       </c>
       <c r="L27" t="n">
-        <v>60.91177234647034</v>
+        <v>60.81302160408029</v>
       </c>
       <c r="M27" t="n">
         <v>30</v>
       </c>
       <c r="N27" t="n">
-        <v>4860546.866097015</v>
+        <v>4850140.581943936</v>
       </c>
       <c r="O27" t="n">
         <v>0</v>
@@ -1890,7 +1890,7 @@
         <v>0.9999999999999999</v>
       </c>
       <c r="Q27" t="n">
-        <v>14581640.59829105</v>
+        <v>14550421.74583181</v>
       </c>
     </row>
     <row r="28">
@@ -1898,52 +1898,52 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>13515445.17887735</v>
+        <v>13488963.45834676</v>
       </c>
       <c r="C28" t="n">
-        <v>5322298818.376231</v>
+        <v>5310903937.22861</v>
       </c>
       <c r="D28" t="n">
-        <v>184364891444.6855</v>
+        <v>184293802595.9931</v>
       </c>
       <c r="E28" t="n">
-        <v>0.6828329312766129</v>
+        <v>0.6825696392444189</v>
       </c>
       <c r="F28" t="n">
-        <v>0.9436217959999318</v>
+        <v>0.9436789700102478</v>
       </c>
       <c r="G28" t="n">
-        <v>85.37946079195133</v>
+        <v>85.25353294751496</v>
       </c>
       <c r="H28" t="n">
-        <v>1501716.130986372</v>
+        <v>1498773.717594085</v>
       </c>
       <c r="I28" t="n">
-        <v>76.07848706525375</v>
+        <v>75.95650836129141</v>
       </c>
       <c r="J28" t="n">
-        <v>59.72854909074773</v>
+        <v>59.64106466827928</v>
       </c>
       <c r="K28" t="n">
-        <v>59.72854909074773</v>
+        <v>59.64106466827928</v>
       </c>
       <c r="L28" t="n">
-        <v>57.56999257187289</v>
+        <v>57.48784477625219</v>
       </c>
       <c r="M28" t="n">
         <v>30</v>
       </c>
       <c r="N28" t="n">
-        <v>4505148.392959117</v>
+        <v>4496321.152782254</v>
       </c>
       <c r="O28" t="n">
         <v>0</v>
       </c>
       <c r="P28" t="n">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="Q28" t="n">
-        <v>13515445.17887735</v>
+        <v>13488963.45834676</v>
       </c>
     </row>
     <row r="29">
@@ -1951,52 +1951,52 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>12516524.74193067</v>
+        <v>12494697.35620288</v>
       </c>
       <c r="C29" t="n">
-        <v>4933137490.290233</v>
+        <v>4923471662.296568</v>
       </c>
       <c r="D29" t="n">
-        <v>189298028934.9757</v>
+        <v>189217274258.2897</v>
       </c>
       <c r="E29" t="n">
-        <v>0.7011038108702804</v>
+        <v>0.7008047194751469</v>
       </c>
       <c r="F29" t="n">
-        <v>0.9458297250639879</v>
+        <v>0.9458791115481638</v>
       </c>
       <c r="G29" t="n">
-        <v>80.64931668408362</v>
+        <v>80.54644387936503</v>
       </c>
       <c r="H29" t="n">
-        <v>1390724.97132563</v>
+        <v>1388299.706244765</v>
       </c>
       <c r="I29" t="n">
-        <v>71.50935120866346</v>
+        <v>71.4102927830921</v>
       </c>
       <c r="J29" t="n">
-        <v>56.46028465322152</v>
+        <v>56.38964004663463</v>
       </c>
       <c r="K29" t="n">
-        <v>56.46028465322149</v>
+        <v>56.38964004663463</v>
       </c>
       <c r="L29" t="n">
-        <v>54.50332315029949</v>
+        <v>54.43708947243343</v>
       </c>
       <c r="M29" t="n">
         <v>30</v>
       </c>
       <c r="N29" t="n">
-        <v>4172174.91397689</v>
+        <v>4164899.118734294</v>
       </c>
       <c r="O29" t="n">
         <v>0</v>
       </c>
       <c r="P29" t="n">
-        <v>0.9999999999999994</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="Q29" t="n">
-        <v>12516524.74193067</v>
+        <v>12494697.35620288</v>
       </c>
     </row>
     <row r="30">
@@ -2004,43 +2004,43 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>11580239.73395392</v>
+        <v>11562865.29415256</v>
       </c>
       <c r="C30" t="n">
-        <v>4568531530.804694</v>
+        <v>4560564535.014051</v>
       </c>
       <c r="D30" t="n">
-        <v>193866560465.7804</v>
+        <v>193777838793.3037</v>
       </c>
       <c r="E30" t="n">
-        <v>0.7180242980214089</v>
+        <v>0.7176956992344582</v>
       </c>
       <c r="F30" t="n">
-        <v>0.9479892146179545</v>
+        <v>0.9480300542660076</v>
       </c>
       <c r="G30" t="n">
-        <v>76.25747804483042</v>
+        <v>76.17640704100256</v>
       </c>
       <c r="H30" t="n">
-        <v>1286693.303772658</v>
+        <v>1284762.810461395</v>
       </c>
       <c r="I30" t="n">
-        <v>67.2942022315826</v>
+        <v>67.21668081075642</v>
       </c>
       <c r="J30" t="n">
-        <v>53.46305134152996</v>
+        <v>53.40810793719938</v>
       </c>
       <c r="K30" t="n">
-        <v>53.46305134152995</v>
+        <v>53.40810793719937</v>
       </c>
       <c r="L30" t="n">
-        <v>51.69544289435019</v>
+        <v>51.6440151461629</v>
       </c>
       <c r="M30" t="n">
         <v>30</v>
       </c>
       <c r="N30" t="n">
-        <v>3860079.911317974</v>
+        <v>3854288.431384185</v>
       </c>
       <c r="O30" t="n">
         <v>0</v>
@@ -2049,7 +2049,7 @@
         <v>0.9999999999999998</v>
       </c>
       <c r="Q30" t="n">
-        <v>11580239.73395392</v>
+        <v>11562865.29415256</v>
       </c>
     </row>
     <row r="31">
@@ -2057,52 +2057,52 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>10702372.9211814</v>
+        <v>10689174.74272567</v>
       </c>
       <c r="C31" t="n">
-        <v>4226787502.893181</v>
+        <v>4220445832.365683</v>
       </c>
       <c r="D31" t="n">
-        <v>198093347968.6736</v>
+        <v>197998284625.6694</v>
       </c>
       <c r="E31" t="n">
-        <v>0.7336790665506429</v>
+        <v>0.7333269800950719</v>
       </c>
       <c r="F31" t="n">
-        <v>0.9500849464355821</v>
+        <v>0.9501169347997442</v>
       </c>
       <c r="G31" t="n">
-        <v>72.183028093818</v>
+        <v>72.12212928446425</v>
       </c>
       <c r="H31" t="n">
-        <v>1189152.546797934</v>
+        <v>1187686.082525074</v>
       </c>
       <c r="I31" t="n">
-        <v>63.4132241570714</v>
+        <v>63.35546898255826</v>
       </c>
       <c r="J31" t="n">
-        <v>50.72124920736379</v>
+        <v>50.68059045787199</v>
       </c>
       <c r="K31" t="n">
-        <v>50.72124920736379</v>
+        <v>50.68059045787197</v>
       </c>
       <c r="L31" t="n">
-        <v>49.13125134269256</v>
+        <v>49.09326149339545</v>
       </c>
       <c r="M31" t="n">
         <v>30</v>
       </c>
       <c r="N31" t="n">
-        <v>3567457.640393801</v>
+        <v>3563058.247575223</v>
       </c>
       <c r="O31" t="n">
         <v>0</v>
       </c>
       <c r="P31" t="n">
-        <v>1</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="Q31" t="n">
-        <v>10702372.9211814</v>
+        <v>10689174.74272567</v>
       </c>
     </row>
     <row r="32">
@@ -2110,43 +2110,43 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>9879068.995415844</v>
+        <v>9869726.55296085</v>
       </c>
       <c r="C32" t="n">
-        <v>3906366116.231212</v>
+        <v>3901548781.09487</v>
       </c>
       <c r="D32" t="n">
-        <v>201999714084.9048</v>
+        <v>201899833406.7643</v>
       </c>
       <c r="E32" t="n">
-        <v>0.748147089203351</v>
+        <v>0.7477771607657936</v>
       </c>
       <c r="F32" t="n">
-        <v>0.9521050275209244</v>
+        <v>0.95212822201833</v>
       </c>
       <c r="G32" t="n">
-        <v>68.40678637259902</v>
+        <v>68.36421395224198</v>
       </c>
       <c r="H32" t="n">
-        <v>1097674.332823983</v>
+        <v>1096636.283662317</v>
       </c>
       <c r="I32" t="n">
-        <v>59.84825886358279</v>
+        <v>59.80827255192713</v>
       </c>
       <c r="J32" t="n">
-        <v>48.22032330794265</v>
+        <v>48.1923779006877</v>
       </c>
       <c r="K32" t="n">
-        <v>48.22032330794265</v>
+        <v>48.1923779006877</v>
       </c>
       <c r="L32" t="n">
-        <v>46.79659732040106</v>
+        <v>46.77053524624316</v>
       </c>
       <c r="M32" t="n">
         <v>30</v>
       </c>
       <c r="N32" t="n">
-        <v>3293022.998471948</v>
+        <v>3289908.85098695</v>
       </c>
       <c r="O32" t="n">
         <v>0</v>
@@ -2155,7 +2155,7 @@
         <v>1</v>
       </c>
       <c r="Q32" t="n">
-        <v>9879068.995415844</v>
+        <v>9869726.55296085</v>
       </c>
     </row>
     <row r="33">
@@ -2163,43 +2163,43 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>9106788.560568172</v>
+        <v>9100960.173394205</v>
       </c>
       <c r="C33" t="n">
-        <v>3605860183.326783</v>
+        <v>3602450191.83071</v>
       </c>
       <c r="D33" t="n">
-        <v>205605574268.2316</v>
+        <v>205502283598.595</v>
       </c>
       <c r="E33" t="n">
-        <v>0.7615021269193761</v>
+        <v>0.7611195688836851</v>
       </c>
       <c r="F33" t="n">
-        <v>0.9540404267696435</v>
+        <v>0.954055162083987</v>
       </c>
       <c r="G33" t="n">
-        <v>64.91105142880697</v>
+        <v>64.88485940859906</v>
       </c>
       <c r="H33" t="n">
-        <v>1011865.395618686</v>
+        <v>1011217.797043801</v>
       </c>
       <c r="I33" t="n">
-        <v>56.58249907855376</v>
+        <v>56.55817521304824</v>
       </c>
       <c r="J33" t="n">
-        <v>45.94653076711557</v>
+        <v>45.92966347770683</v>
       </c>
       <c r="K33" t="n">
-        <v>45.94653076711558</v>
+        <v>45.92966347770684</v>
       </c>
       <c r="L33" t="n">
-        <v>44.67806203836976</v>
+        <v>44.66236246376257</v>
       </c>
       <c r="M33" t="n">
         <v>30</v>
       </c>
       <c r="N33" t="n">
-        <v>3035596.186856057</v>
+        <v>3033653.391131402</v>
       </c>
       <c r="O33" t="n">
         <v>0</v>
@@ -2208,7 +2208,7 @@
         <v>1</v>
       </c>
       <c r="Q33" t="n">
-        <v>9106788.560568172</v>
+        <v>9100960.173394205</v>
       </c>
     </row>
     <row r="34">
@@ -2216,43 +2216,43 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>8382273.199697859</v>
+        <v>8379612.159456227</v>
       </c>
       <c r="C34" t="n">
-        <v>3323977824.607383</v>
+        <v>3321850463.288885</v>
       </c>
       <c r="D34" t="n">
-        <v>208929552092.839</v>
+        <v>208824134061.8839</v>
       </c>
       <c r="E34" t="n">
-        <v>0.7738131558994036</v>
+        <v>0.7734227187477181</v>
       </c>
       <c r="F34" t="n">
-        <v>0.9558845040238724</v>
+        <v>0.9558913182575018</v>
       </c>
       <c r="G34" t="n">
-        <v>61.67939680257022</v>
+        <v>61.66762212081809</v>
       </c>
       <c r="H34" t="n">
-        <v>931363.6888553177</v>
+        <v>931068.0177173585</v>
       </c>
       <c r="I34" t="n">
-        <v>53.60022668863996</v>
+        <v>53.58943552901686</v>
       </c>
       <c r="J34" t="n">
-        <v>43.88675243551789</v>
+        <v>43.8793309432603</v>
       </c>
       <c r="K34" t="n">
-        <v>43.88675243551789</v>
+        <v>43.8793309432603</v>
       </c>
       <c r="L34" t="n">
-        <v>42.76278769460964</v>
+        <v>42.75589411871023</v>
       </c>
       <c r="M34" t="n">
         <v>30</v>
       </c>
       <c r="N34" t="n">
-        <v>2794091.066565953</v>
+        <v>2793204.053152076</v>
       </c>
       <c r="O34" t="n">
         <v>0</v>
@@ -2261,7 +2261,7 @@
         <v>1</v>
       </c>
       <c r="Q34" t="n">
-        <v>8382273.199697859</v>
+        <v>8379612.159456227</v>
       </c>
     </row>
     <row r="35">
@@ -2269,52 +2269,52 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>7702519.099167037</v>
+        <v>7702684.861423682</v>
       </c>
       <c r="C35" t="n">
-        <v>3059529717.889719</v>
+        <v>3058558438.201523</v>
       </c>
       <c r="D35" t="n">
-        <v>211989081810.7287</v>
+        <v>211882692500.0854</v>
       </c>
       <c r="E35" t="n">
-        <v>0.7851447474471432</v>
+        <v>0.7847507129632793</v>
       </c>
       <c r="F35" t="n">
-        <v>0.957632615293178</v>
+        <v>0.9576321874863704</v>
       </c>
       <c r="G35" t="n">
-        <v>58.69650732843204</v>
+        <v>58.69722831792983</v>
       </c>
       <c r="H35" t="n">
-        <v>855835.4554630041</v>
+        <v>855853.8734915203</v>
       </c>
       <c r="I35" t="n">
-        <v>50.88658484407922</v>
+        <v>50.88723551850369</v>
       </c>
       <c r="J35" t="n">
-        <v>42.02834272320979</v>
+        <v>42.02878635452922</v>
       </c>
       <c r="K35" t="n">
-        <v>42.0283427232098</v>
+        <v>42.02878635452922</v>
       </c>
       <c r="L35" t="n">
-        <v>41.038345449337</v>
+        <v>41.03875665808012</v>
       </c>
       <c r="M35" t="n">
         <v>30</v>
       </c>
       <c r="N35" t="n">
-        <v>2567506.366389012</v>
+        <v>2567561.620474561</v>
       </c>
       <c r="O35" t="n">
         <v>0</v>
       </c>
       <c r="P35" t="n">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="Q35" t="n">
-        <v>7702519.099167037</v>
+        <v>7702684.861423682</v>
       </c>
     </row>
     <row r="36">
@@ -2322,43 +2322,43 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>7064757.283939565</v>
+        <v>7067422.928163984</v>
       </c>
       <c r="C36" t="n">
-        <v>2811419471.195969</v>
+        <v>2811479974.419644</v>
       </c>
       <c r="D36" t="n">
-        <v>214800501281.9246</v>
+        <v>214694172474.505</v>
       </c>
       <c r="E36" t="n">
-        <v>0.7955574121552764</v>
+        <v>0.7951636017574261</v>
       </c>
       <c r="F36" t="n">
-        <v>0.9592817813794469</v>
+        <v>0.9592748800076143</v>
       </c>
       <c r="G36" t="n">
-        <v>55.94804578469679</v>
+        <v>55.9594221530901</v>
       </c>
       <c r="H36" t="n">
-        <v>784973.0315488405</v>
+        <v>785269.2142404426</v>
       </c>
       <c r="I36" t="n">
-        <v>48.42737650934322</v>
+        <v>48.43746188093785</v>
       </c>
       <c r="J36" t="n">
-        <v>40.35901349242779</v>
+        <v>40.36582820900532</v>
       </c>
       <c r="K36" t="n">
-        <v>40.35901349242779</v>
+        <v>40.36582820900533</v>
       </c>
       <c r="L36" t="n">
-        <v>39.49263848997751</v>
+        <v>39.4989417003398</v>
       </c>
       <c r="M36" t="n">
         <v>30</v>
       </c>
       <c r="N36" t="n">
-        <v>2354919.094646521</v>
+        <v>2355807.642721328</v>
       </c>
       <c r="O36" t="n">
         <v>0</v>
@@ -2367,7 +2367,7 @@
         <v>1</v>
       </c>
       <c r="Q36" t="n">
-        <v>7064757.283939565</v>
+        <v>7067422.928163984</v>
       </c>
     </row>
     <row r="37">
@@ -2375,43 +2375,43 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>6466438.944829221</v>
+        <v>6471295.808125961</v>
       </c>
       <c r="C37" t="n">
-        <v>2578636408.637941</v>
+        <v>2579609368.779854</v>
       </c>
       <c r="D37" t="n">
-        <v>217379137690.5626</v>
+        <v>217273781843.2849</v>
       </c>
       <c r="E37" t="n">
-        <v>0.8051079173724539</v>
+        <v>0.8047177105306847</v>
       </c>
       <c r="F37" t="n">
-        <v>0.9608304097426932</v>
+        <v>0.960817851256234</v>
       </c>
       <c r="G37" t="n">
-        <v>53.42054222283691</v>
+        <v>53.44084119033932</v>
       </c>
       <c r="H37" t="n">
-        <v>718493.2160921356</v>
+        <v>719032.8675695512</v>
       </c>
       <c r="I37" t="n">
-        <v>46.20888567461636</v>
+        <v>46.22651446476921</v>
       </c>
       <c r="J37" t="n">
-        <v>38.86674927165658</v>
+        <v>38.87855203285927</v>
       </c>
       <c r="K37" t="n">
-        <v>38.86674927165659</v>
+        <v>38.87855203285927</v>
       </c>
       <c r="L37" t="n">
-        <v>38.11383682594197</v>
+        <v>38.12473040647455</v>
       </c>
       <c r="M37" t="n">
         <v>30</v>
       </c>
       <c r="N37" t="n">
-        <v>2155479.648276407</v>
+        <v>2157098.602708654</v>
       </c>
       <c r="O37" t="n">
         <v>0</v>
@@ -2420,7 +2420,7 @@
         <v>1</v>
       </c>
       <c r="Q37" t="n">
-        <v>6466438.944829221</v>
+        <v>6471295.808125961</v>
       </c>
     </row>
     <row r="38">
@@ -2428,43 +2428,43 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>5905224.647722953</v>
+        <v>5911984.819127208</v>
       </c>
       <c r="C38" t="n">
-        <v>2360250214.862666</v>
+        <v>2362022969.965976</v>
       </c>
       <c r="D38" t="n">
-        <v>219739387905.4252</v>
+        <v>219635804813.2509</v>
       </c>
       <c r="E38" t="n">
-        <v>0.8138495848349082</v>
+        <v>0.8134659437527809</v>
       </c>
       <c r="F38" t="n">
-        <v>0.9622780614103833</v>
+        <v>0.9622606776243945</v>
       </c>
       <c r="G38" t="n">
-        <v>51.10130008061746</v>
+        <v>51.12891221454087</v>
       </c>
       <c r="H38" t="n">
-        <v>656136.071969217</v>
+        <v>656887.2021252452</v>
       </c>
       <c r="I38" t="n">
-        <v>44.21772040664351</v>
+        <v>44.24113992786557</v>
       </c>
       <c r="J38" t="n">
-        <v>37.53975158399068</v>
+        <v>37.55528636190054</v>
       </c>
       <c r="K38" t="n">
-        <v>37.53975158399068</v>
+        <v>37.55528636190055</v>
       </c>
       <c r="L38" t="n">
-        <v>36.89034061895089</v>
+        <v>36.90464855595521</v>
       </c>
       <c r="M38" t="n">
         <v>30</v>
       </c>
       <c r="N38" t="n">
-        <v>1968408.215907651</v>
+        <v>1970661.606375736</v>
       </c>
       <c r="O38" t="n">
         <v>0</v>
@@ -2473,7 +2473,7 @@
         <v>1</v>
       </c>
       <c r="Q38" t="n">
-        <v>5905224.647722953</v>
+        <v>5911984.819127208</v>
       </c>
     </row>
     <row r="39">
@@ -2481,52 +2481,52 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>5378976.428484837</v>
+        <v>5387373.629206004</v>
       </c>
       <c r="C39" t="n">
-        <v>2155406996.418878</v>
+        <v>2157874458.981431</v>
       </c>
       <c r="D39" t="n">
-        <v>221894794901.8441</v>
+        <v>221793679272.2323</v>
       </c>
       <c r="E39" t="n">
-        <v>0.8218325737105338</v>
+        <v>0.8214580713786381</v>
       </c>
       <c r="F39" t="n">
-        <v>0.9636252562291374</v>
+        <v>0.9636038692907165</v>
       </c>
       <c r="G39" t="n">
-        <v>48.9783145615513</v>
+        <v>49.01176202624865</v>
       </c>
       <c r="H39" t="n">
-        <v>597664.0476094263</v>
+        <v>598597.0699117782</v>
       </c>
       <c r="I39" t="n">
-        <v>42.4406791849617</v>
+        <v>42.4682910770595</v>
       </c>
       <c r="J39" t="n">
-        <v>36.36641001551453</v>
+        <v>36.38455714374748</v>
       </c>
       <c r="K39" t="n">
-        <v>36.36641001551453</v>
+        <v>36.38455714374747</v>
       </c>
       <c r="L39" t="n">
-        <v>35.8107684732436</v>
+        <v>35.82744822242891</v>
       </c>
       <c r="M39" t="n">
         <v>30</v>
       </c>
       <c r="N39" t="n">
-        <v>1792992.142828279</v>
+        <v>1795791.209735335</v>
       </c>
       <c r="O39" t="n">
         <v>0</v>
       </c>
       <c r="P39" t="n">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="Q39" t="n">
-        <v>5378976.428484837</v>
+        <v>5387373.629206004</v>
       </c>
     </row>
     <row r="40">
@@ -2534,43 +2534,43 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>4885751.909433925</v>
+        <v>4895541.164451643</v>
       </c>
       <c r="C40" t="n">
-        <v>1963326396.396965</v>
+        <v>1966391374.660191</v>
       </c>
       <c r="D40" t="n">
-        <v>223858121298.2411</v>
+        <v>223760070646.8925</v>
       </c>
       <c r="E40" t="n">
-        <v>0.8291041529564485</v>
+        <v>0.8287410023958981</v>
       </c>
       <c r="F40" t="n">
-        <v>0.9648733109005816</v>
+        <v>0.9648487145885004</v>
       </c>
       <c r="G40" t="n">
-        <v>47.04019985330345</v>
+        <v>47.07813917497324</v>
       </c>
       <c r="H40" t="n">
-        <v>542861.323270436</v>
+        <v>543949.0182724048</v>
       </c>
       <c r="I40" t="n">
-        <v>40.86464338481732</v>
+        <v>40.89501399811162</v>
       </c>
       <c r="J40" t="n">
-        <v>35.33529699387448</v>
+        <v>35.35507713029426</v>
       </c>
       <c r="K40" t="n">
-        <v>35.33529699387448</v>
+        <v>35.35507713029426</v>
       </c>
       <c r="L40" t="n">
-        <v>34.86396644162679</v>
+        <v>34.88211145844002</v>
       </c>
       <c r="M40" t="n">
         <v>30</v>
       </c>
       <c r="N40" t="n">
-        <v>1628583.969811308</v>
+        <v>1631847.054817214</v>
       </c>
       <c r="O40" t="n">
         <v>0</v>
@@ -2579,7 +2579,7 @@
         <v>1</v>
       </c>
       <c r="Q40" t="n">
-        <v>4885751.909433925</v>
+        <v>4895541.164451643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>